<commit_message>
Adapted ranges for Huawei 4G and 5G
</commit_message>
<xml_diff>
--- a/output/template_single.xlsx
+++ b/output/template_single.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://diuoagr-my.sharepoint.com/personal/grad0909_di_uoa_gr/Documents/Surecom/Surecom_KPI/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_AD4DCBB4A06381AAC71CFC7EF616CCC8683EDF1C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EA5851B6-ECAF-41C5-AAF2-7D75DE75D151}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_AD4DCBB4A06381AAC71CFC7EF616CCC8683EDF1C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E9449BC2-D03B-4C1F-89A5-C5A8C7777D1F}"/>
   <bookViews>
-    <workbookView xWindow="30480" yWindow="1245" windowWidth="21600" windowHeight="12855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input3G" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>UMTS RSCP (dBm)</t>
   </si>
@@ -64,24 +64,9 @@
     <t>Coverage Level</t>
   </si>
   <si>
-    <t>Poor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reasonable </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good </t>
-  </si>
-  <si>
     <t>Quality Level</t>
   </si>
   <si>
-    <t>-15 to -34</t>
-  </si>
-  <si>
-    <t>0 to -14</t>
-  </si>
-  <si>
     <t>Band</t>
   </si>
   <si>
@@ -92,13 +77,61 @@
   </si>
   <si>
     <t>Vodafone:input\VF BMT Car pk UMTS.FMT</t>
+  </si>
+  <si>
+    <t>&lt;= -110</t>
+  </si>
+  <si>
+    <t>-110 to -105</t>
+  </si>
+  <si>
+    <t>-105 to -100</t>
+  </si>
+  <si>
+    <t>-100 to -95</t>
+  </si>
+  <si>
+    <t>-95 to -90</t>
+  </si>
+  <si>
+    <t>-90 to -85</t>
+  </si>
+  <si>
+    <t>-85 to -80</t>
+  </si>
+  <si>
+    <t>-80 to -75</t>
+  </si>
+  <si>
+    <t>-75 to -70</t>
+  </si>
+  <si>
+    <t>&gt;= -70</t>
+  </si>
+  <si>
+    <t>&lt;= -13</t>
+  </si>
+  <si>
+    <t>-13 to -10</t>
+  </si>
+  <si>
+    <t>-10 to -7</t>
+  </si>
+  <si>
+    <t>-7 to -4</t>
+  </si>
+  <si>
+    <t>&gt;= -4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,20 +147,35 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <color theme="1" tint="0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,24 +196,90 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF6CD1E"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF38F729"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF48F836"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CC33"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF006600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF48F836"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CC33"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -175,14 +289,29 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -192,104 +321,11 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -304,124 +340,157 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{BEEDB7A1-CA4B-455D-A8E7-57769FF3FC87}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -801,7 +870,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -811,19 +880,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC13D29-B219-4AE5-9192-3696E6318D31}">
-  <dimension ref="B2:E16"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
         <v>10</v>
       </c>
@@ -831,150 +901,220 @@
       <c r="D2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="4">
+    </row>
+    <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="1">
         <f>Input3G!C2</f>
         <v>0.53467199463279902</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4">
+    <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="1">
         <f>Input3G!C3</f>
         <v>0.186763260574031</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
-        <v>3</v>
+    <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="C5" s="22"/>
-      <c r="D5" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="24">
+      <c r="D5" s="1">
         <f>Input3G!C4</f>
         <v>0.27856474479316801</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="str">
+    <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="1">
+        <f>Input3G!C5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="1">
+        <f>Input3G!C6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="1">
+        <f>Input3G!C7</f>
+        <v>0.22688778903137299</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="1">
+        <f>Input3G!C8</f>
+        <v>0.77311221096862603</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="27"/>
+      <c r="D10" s="1">
+        <f>Input3G!C9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="1">
+        <f>Input3G!C10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="1">
+        <f>Input3G!C11</f>
+        <v>0.43500803314481401</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="str">
         <f>Input3G!A14</f>
         <v>Vodafone:input\VF BMT Car pk UMTS.FMT</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="20"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="11">
+    </row>
+    <row r="16" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="31"/>
+      <c r="D16" s="1">
         <f>Input3G!C7</f>
         <v>0.22688778903137299</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="11">
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="32"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="35"/>
+      <c r="D20" s="1">
         <f>Input3G!C8</f>
         <v>0.77311221096862603</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="25" t="str">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="str">
         <f>Input3G!A14</f>
         <v>Vodafone:input\VF BMT Car pk UMTS.FMT</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="C21" s="15"/>
+      <c r="D21" s="30"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="7">
+      <c r="C24" s="8"/>
+      <c r="D24" s="1">
         <f>Input3G!C11</f>
         <v>0.43500803314481401</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="7">
+      <c r="C25" s="8"/>
+      <c r="D25" s="1">
         <f>Input3G!C12</f>
         <v>0.56499196685518505</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="28" t="str">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="str">
         <f>Input3G!A14</f>
         <v>Vodafone:input\VF BMT Car pk UMTS.FMT</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="30"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B16:D16"/>
+  <mergeCells count="8">
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B2:C2"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixes for single excel template
</commit_message>
<xml_diff>
--- a/output/template_single.xlsx
+++ b/output/template_single.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://diuoagr-my.sharepoint.com/personal/grad0909_di_uoa_gr/Documents/Surecom/Surecom_KPI/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_AD4DCBB4A06381AAC71CFC7EF616CCC8683EDF1C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E9449BC2-D03B-4C1F-89A5-C5A8C7777D1F}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_AD4DCBB4A06381AAC71CFC7EF616CCC8683EDF1C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1D135FF7-CDAA-4E3C-8A83-273B9DBE3E8A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,29 +26,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>UMTS RSCP (dBm)</t>
   </si>
   <si>
-    <t>&lt;= -101</t>
-  </si>
-  <si>
-    <t>-94 to -101</t>
-  </si>
-  <si>
-    <t>-15 to -94</t>
-  </si>
-  <si>
     <t>UMTS Ec/Io (dB)</t>
   </si>
   <si>
-    <t>-34 to -14</t>
-  </si>
-  <si>
-    <t>-14 to 0</t>
-  </si>
-  <si>
     <t>UMTS Band</t>
   </si>
   <si>
@@ -122,6 +107,39 @@
   </si>
   <si>
     <t>&gt;= -4</t>
+  </si>
+  <si>
+    <t>-105 to -110</t>
+  </si>
+  <si>
+    <t>-100 to -105</t>
+  </si>
+  <si>
+    <t>-95 to -100</t>
+  </si>
+  <si>
+    <t>-90 to -95</t>
+  </si>
+  <si>
+    <t>-85 to -90</t>
+  </si>
+  <si>
+    <t>-80 to -85</t>
+  </si>
+  <si>
+    <t>-75 to -80</t>
+  </si>
+  <si>
+    <t>-70 to -75</t>
+  </si>
+  <si>
+    <t>-15 to -70</t>
+  </si>
+  <si>
+    <t>-34 to -13</t>
+  </si>
+  <si>
+    <t>-4 to 0</t>
   </si>
 </sst>
 </file>
@@ -421,47 +439,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -479,14 +458,53 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A14"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,94 +801,204 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>90852</v>
+        <v>50954</v>
       </c>
       <c r="C2">
-        <v>0.53467199463279902</v>
+        <v>0.29986876254259298</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B3">
-        <v>31735</v>
+        <v>21024</v>
       </c>
       <c r="C3">
-        <v>0.186763260574031</v>
+        <v>0.12372808540439301</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B4">
-        <v>47334</v>
+        <v>24977</v>
       </c>
       <c r="C4">
-        <v>0.27856474479316801</v>
+        <v>0.146991837383254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>21874</v>
+      </c>
+      <c r="C5">
+        <v>0.12873041001406499</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>15455</v>
+      </c>
+      <c r="C6">
+        <v>9.0954031579381006E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B7">
-        <v>38553</v>
+        <v>14374</v>
       </c>
       <c r="C7">
-        <v>0.22688778903137299</v>
+        <v>8.4592251693433998E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B8">
-        <v>131368</v>
+        <v>12801</v>
       </c>
       <c r="C8">
-        <v>0.77311221096862603</v>
+        <v>7.5335008621653599E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>6249</v>
+      </c>
+      <c r="C9">
+        <v>3.6775913512750003E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>2144</v>
+      </c>
+      <c r="C10">
+        <v>1.2617628191924401E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B11">
-        <v>73917</v>
+        <v>69</v>
       </c>
       <c r="C11">
-        <v>0.43500803314481401</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>96004</v>
-      </c>
-      <c r="C12">
-        <v>0.56499196685518505</v>
+        <v>4.06071056549808E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>36</v>
+      </c>
+      <c r="B14">
+        <v>44872</v>
+      </c>
+      <c r="C14">
+        <v>0.26407565868844901</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>23066</v>
+      </c>
+      <c r="C15">
+        <v>0.135745434643157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>30029</v>
+      </c>
+      <c r="C16">
+        <v>0.176723300828031</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>50225</v>
+      </c>
+      <c r="C17">
+        <v>0.29557853355382702</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18">
+        <v>21729</v>
+      </c>
+      <c r="C18">
+        <v>0.127877072286533</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>73917</v>
+      </c>
+      <c r="C21">
+        <v>0.43500803314481401</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>96004</v>
+      </c>
+      <c r="C22">
+        <v>0.56499196685518505</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -883,7 +1011,7 @@
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,216 +1022,225 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18" t="s">
-        <v>11</v>
+      <c r="B2" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="20"/>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7"/>
       <c r="D3" s="1">
         <f>Input3G!C2</f>
-        <v>0.53467199463279902</v>
+        <v>0.29986876254259298</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="21"/>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8"/>
       <c r="D4" s="1">
         <f>Input3G!C3</f>
-        <v>0.186763260574031</v>
+        <v>0.12372808540439301</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="22"/>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="9"/>
       <c r="D5" s="1">
         <f>Input3G!C4</f>
-        <v>0.27856474479316801</v>
+        <v>0.146991837383254</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="23"/>
+      <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="10"/>
       <c r="D6" s="1">
         <f>Input3G!C5</f>
-        <v>0</v>
+        <v>0.12873041001406499</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="24"/>
+      <c r="B7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="11"/>
       <c r="D7" s="1">
         <f>Input3G!C6</f>
-        <v>0</v>
+        <v>9.0954031579381006E-2</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="25"/>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="12"/>
       <c r="D8" s="1">
         <f>Input3G!C7</f>
-        <v>0.22688778903137299</v>
+        <v>8.4592251693433998E-2</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="26"/>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="13"/>
       <c r="D9" s="1">
         <f>Input3G!C8</f>
-        <v>0.77311221096862603</v>
+        <v>7.5335008621653599E-2</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="27"/>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="14"/>
       <c r="D10" s="1">
         <f>Input3G!C9</f>
-        <v>0</v>
+        <v>3.6775913512750003E-2</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="28"/>
+      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="15"/>
       <c r="D11" s="1">
         <f>Input3G!C10</f>
-        <v>0</v>
+        <v>1.2617628191924401E-2</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="29"/>
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="16"/>
       <c r="D12" s="1">
         <f>Input3G!C11</f>
-        <v>0.43500803314481401</v>
+        <v>4.06071056549808E-4</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="str">
-        <f>Input3G!A14</f>
+      <c r="B13" s="30" t="str">
+        <f>Input3G!A24</f>
         <v>Vodafone:input\VF BMT Car pk UMTS.FMT</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="13" t="s">
-        <v>12</v>
+      <c r="B15" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="31"/>
+        <v>22</v>
+      </c>
+      <c r="C16" s="17"/>
       <c r="D16" s="1">
-        <f>Input3G!C7</f>
-        <v>0.22688778903137299</v>
+        <f>Input3G!C14</f>
+        <v>0.26407565868844901</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="1">
+        <f>Input3G!C15</f>
+        <v>0.135745434643157</v>
+      </c>
     </row>
     <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="1">
+        <f>Input3G!C16</f>
+        <v>0.176723300828031</v>
+      </c>
     </row>
     <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="1">
+        <f>Input3G!C17</f>
+        <v>0.29557853355382702</v>
+      </c>
     </row>
     <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="35"/>
+        <v>26</v>
+      </c>
+      <c r="C20" s="21"/>
       <c r="D20" s="1">
-        <f>Input3G!C8</f>
-        <v>0.77311221096862603</v>
+        <f>Input3G!C18</f>
+        <v>0.127877072286533</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="str">
-        <f>Input3G!A14</f>
+      <c r="B21" s="33" t="str">
+        <f>Input3G!A24</f>
         <v>Vodafone:input\VF BMT Car pk UMTS.FMT</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="30"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="35"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="9"/>
+      <c r="B23" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="29"/>
       <c r="D23" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="8"/>
+      <c r="B24" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="26"/>
       <c r="D24" s="1">
-        <f>Input3G!C11</f>
+        <f>Input3G!C21</f>
         <v>0.43500803314481401</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="8"/>
+      <c r="B25" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="26"/>
       <c r="D25" s="1">
-        <f>Input3G!C12</f>
+        <f>Input3G!C22</f>
         <v>0.56499196685518505</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="str">
-        <f>Input3G!A14</f>
+      <c r="B26" s="22" t="str">
+        <f>Input3G!A24</f>
         <v>Vodafone:input\VF BMT Car pk UMTS.FMT</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Change names on excel sheets
</commit_message>
<xml_diff>
--- a/output/template_single.xlsx
+++ b/output/template_single.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://diuoagr-my.sharepoint.com/personal/grad0909_di_uoa_gr/Documents/Surecom/Surecom_KPI/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_AD4DCBB4A06381AAC71CFC7EF616CCC8683EDF1C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1D135FF7-CDAA-4E3C-8A83-273B9DBE3E8A}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_AD4DCBB4A06381AAC71CFC7EF616CCC8683EDF1C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D38448D2-E62D-4131-86E6-CEE61C3A84D5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Input3G" sheetId="1" r:id="rId1"/>
-    <sheet name="Output3G" sheetId="2" r:id="rId2"/>
+    <sheet name="Input4G_5G" sheetId="1" r:id="rId1"/>
+    <sheet name="Output4G_5G" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1011,7 +1011,7 @@
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="1">
-        <f>Input3G!C2</f>
+        <f>Input4G_5G!C2</f>
         <v>0.29986876254259298</v>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="1">
-        <f>Input3G!C3</f>
+        <f>Input4G_5G!C3</f>
         <v>0.12372808540439301</v>
       </c>
     </row>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="1">
-        <f>Input3G!C4</f>
+        <f>Input4G_5G!C4</f>
         <v>0.146991837383254</v>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="1">
-        <f>Input3G!C5</f>
+        <f>Input4G_5G!C5</f>
         <v>0.12873041001406499</v>
       </c>
     </row>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="1">
-        <f>Input3G!C6</f>
+        <f>Input4G_5G!C6</f>
         <v>9.0954031579381006E-2</v>
       </c>
     </row>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="1">
-        <f>Input3G!C7</f>
+        <f>Input4G_5G!C7</f>
         <v>8.4592251693433998E-2</v>
       </c>
     </row>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="1">
-        <f>Input3G!C8</f>
+        <f>Input4G_5G!C8</f>
         <v>7.5335008621653599E-2</v>
       </c>
     </row>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="1">
-        <f>Input3G!C9</f>
+        <f>Input4G_5G!C9</f>
         <v>3.6775913512750003E-2</v>
       </c>
     </row>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="1">
-        <f>Input3G!C10</f>
+        <f>Input4G_5G!C10</f>
         <v>1.2617628191924401E-2</v>
       </c>
     </row>
@@ -1126,13 +1126,13 @@
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="1">
-        <f>Input3G!C11</f>
+        <f>Input4G_5G!C11</f>
         <v>4.06071056549808E-4</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="30" t="str">
-        <f>Input3G!A24</f>
+        <f>Input4G_5G!A24</f>
         <v>Vodafone:input\VF BMT Car pk UMTS.FMT</v>
       </c>
       <c r="C13" s="31"/>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="1">
-        <f>Input3G!C14</f>
+        <f>Input4G_5G!C14</f>
         <v>0.26407565868844901</v>
       </c>
     </row>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="1">
-        <f>Input3G!C15</f>
+        <f>Input4G_5G!C15</f>
         <v>0.135745434643157</v>
       </c>
     </row>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="1">
-        <f>Input3G!C16</f>
+        <f>Input4G_5G!C16</f>
         <v>0.176723300828031</v>
       </c>
     </row>
@@ -1183,7 +1183,7 @@
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="1">
-        <f>Input3G!C17</f>
+        <f>Input4G_5G!C17</f>
         <v>0.29557853355382702</v>
       </c>
     </row>
@@ -1193,13 +1193,13 @@
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="1">
-        <f>Input3G!C18</f>
+        <f>Input4G_5G!C18</f>
         <v>0.127877072286533</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="33" t="str">
-        <f>Input3G!A24</f>
+        <f>Input4G_5G!A24</f>
         <v>Vodafone:input\VF BMT Car pk UMTS.FMT</v>
       </c>
       <c r="C21" s="34"/>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="C24" s="26"/>
       <c r="D24" s="1">
-        <f>Input3G!C21</f>
+        <f>Input4G_5G!C21</f>
         <v>0.43500803314481401</v>
       </c>
     </row>
@@ -1230,13 +1230,13 @@
       </c>
       <c r="C25" s="26"/>
       <c r="D25" s="1">
-        <f>Input3G!C22</f>
+        <f>Input4G_5G!C22</f>
         <v>0.56499196685518505</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="22" t="str">
-        <f>Input3G!A24</f>
+        <f>Input4G_5G!A24</f>
         <v>Vodafone:input\VF BMT Car pk UMTS.FMT</v>
       </c>
       <c r="C26" s="23"/>

</xml_diff>

<commit_message>
New single template file
</commit_message>
<xml_diff>
--- a/output/template_single.xlsx
+++ b/output/template_single.xlsx
@@ -789,7 +789,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection sqref="A1:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,7 +1011,7 @@
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ranges and single template for 3g Huawei
</commit_message>
<xml_diff>
--- a/output/template_single.xlsx
+++ b/output/template_single.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://diuoagr-my.sharepoint.com/personal/grad0909_di_uoa_gr/Documents/Surecom/Surecom_KPI/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_AD4DCBB4A06381AAC71CFC7EF616CCC8683EDF1C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D38448D2-E62D-4131-86E6-CEE61C3A84D5}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="11_AD4DCBB4A06381AAC71CFC7EF616CCC8683EDF1C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BA3D4EB4-EED0-4BA3-B0D9-42D22E7CBCFF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5250" yWindow="3780" windowWidth="21600" windowHeight="12855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Input4G_5G" sheetId="1" r:id="rId1"/>
-    <sheet name="Output4G_5G" sheetId="2" r:id="rId2"/>
+    <sheet name="Input3G" sheetId="1" r:id="rId1"/>
+    <sheet name="Output3G" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>UMTS RSCP (dBm)</t>
   </si>
@@ -61,24 +61,9 @@
     <t>UMTS  Ec/Io (dB)</t>
   </si>
   <si>
-    <t>Vodafone:input\VF BMT Car pk UMTS.FMT</t>
-  </si>
-  <si>
     <t>&lt;= -110</t>
   </si>
   <si>
-    <t>-110 to -105</t>
-  </si>
-  <si>
-    <t>-105 to -100</t>
-  </si>
-  <si>
-    <t>-100 to -95</t>
-  </si>
-  <si>
-    <t>-95 to -90</t>
-  </si>
-  <si>
     <t>-90 to -85</t>
   </si>
   <si>
@@ -91,9 +76,6 @@
     <t>-75 to -70</t>
   </si>
   <si>
-    <t>&gt;= -70</t>
-  </si>
-  <si>
     <t>&lt;= -13</t>
   </si>
   <si>
@@ -109,18 +91,6 @@
     <t>&gt;= -4</t>
   </si>
   <si>
-    <t>-105 to -110</t>
-  </si>
-  <si>
-    <t>-100 to -105</t>
-  </si>
-  <si>
-    <t>-95 to -100</t>
-  </si>
-  <si>
-    <t>-90 to -95</t>
-  </si>
-  <si>
     <t>-85 to -90</t>
   </si>
   <si>
@@ -133,13 +103,40 @@
     <t>-70 to -75</t>
   </si>
   <si>
-    <t>-15 to -70</t>
-  </si>
-  <si>
     <t>-34 to -13</t>
   </si>
   <si>
     <t>-4 to 0</t>
+  </si>
+  <si>
+    <t>&lt;= -90</t>
+  </si>
+  <si>
+    <t>-70 to -65</t>
+  </si>
+  <si>
+    <t>-65 to -60</t>
+  </si>
+  <si>
+    <t>-60 to -55</t>
+  </si>
+  <si>
+    <t>&gt;= -55</t>
+  </si>
+  <si>
+    <t>-65 to -70</t>
+  </si>
+  <si>
+    <t>-60 to -65</t>
+  </si>
+  <si>
+    <t>-55 to -60</t>
+  </si>
+  <si>
+    <t>-15 to -55</t>
+  </si>
+  <si>
+    <t>Eir:input\ccd eir UMTS L1.FMT</t>
   </si>
 </sst>
 </file>
@@ -193,7 +190,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,12 +248,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,7 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -457,12 +448,11 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -786,7 +776,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
@@ -801,204 +791,193 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>50954</v>
+        <v>1901</v>
       </c>
       <c r="C2">
-        <v>0.29986876254259298</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>21024</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.12372808540439301</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <v>24977</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.146991837383254</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B5">
-        <v>21874</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0.12873041001406499</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B6">
-        <v>15455</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>9.0954031579381006E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7">
-        <v>14374</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>8.4592251693433998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8">
-        <v>12801</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>7.5335008621653599E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9">
-        <v>6249</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>3.6775913512750003E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10">
-        <v>2144</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1.2617628191924401E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11">
-        <v>69</v>
-      </c>
-      <c r="C11">
-        <v>4.06071056549808E-4</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>175</v>
+      </c>
+      <c r="C13">
+        <v>9.2056812204103097E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>44872</v>
+        <v>1726</v>
       </c>
       <c r="C14">
-        <v>0.26407565868844901</v>
+        <v>0.907943187795896</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B15">
-        <v>23066</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>0.135745434643157</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B16">
-        <v>30029</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>0.176723300828031</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17">
-        <v>50225</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>0.29557853355382702</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18">
-        <v>21729</v>
-      </c>
-      <c r="C18">
-        <v>0.127877072286533</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>1901</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B21">
-        <v>73917</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>0.43500803314481401</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22">
-        <v>96004</v>
-      </c>
-      <c r="C22">
-        <v>0.56499196685518505</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>11</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1008,10 +987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC13D29-B219-4AE5-9192-3696E6318D31}">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,236 +1001,226 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="27"/>
       <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="1">
-        <f>Input4G_5G!C2</f>
-        <v>0.29986876254259298</v>
+        <f>Input3G!C2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="1">
-        <f>Input4G_5G!C3</f>
-        <v>0.12372808540439301</v>
+        <f>Input3G!C3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="1">
-        <f>Input4G_5G!C4</f>
-        <v>0.146991837383254</v>
+        <f>Input3G!C4</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="1">
-        <f>Input4G_5G!C5</f>
-        <v>0.12873041001406499</v>
+        <f>Input3G!C5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="1">
-        <f>Input4G_5G!C6</f>
-        <v>9.0954031579381006E-2</v>
+        <f>Input3G!C6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="1">
-        <f>Input4G_5G!C7</f>
-        <v>8.4592251693433998E-2</v>
+        <f>Input3G!C7</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="1">
-        <f>Input4G_5G!C8</f>
-        <v>7.5335008621653599E-2</v>
+        <f>Input3G!C8</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="1">
-        <f>Input4G_5G!C9</f>
-        <v>3.6775913512750003E-2</v>
+        <f>Input3G!C9</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="1">
-        <f>Input4G_5G!C10</f>
-        <v>1.2617628191924401E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="1">
-        <f>Input4G_5G!C11</f>
-        <v>4.06071056549808E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="30" t="str">
-        <f>Input4G_5G!A24</f>
-        <v>Vodafone:input\VF BMT Car pk UMTS.FMT</v>
-      </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="29" t="s">
+        <f>Input3G!C11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="29" t="str">
+        <f>Input3G!A23</f>
+        <v>Eir:input\ccd eir UMTS L1.FMT</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="31"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="4" t="s">
+      <c r="C14" s="28"/>
+      <c r="D14" s="4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="1">
+        <f>Input3G!C13</f>
+        <v>9.2056812204103097E-2</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="1">
-        <f>Input4G_5G!C14</f>
-        <v>0.26407565868844901</v>
+        <f>Input3G!C14</f>
+        <v>0.907943187795896</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="1">
-        <f>Input4G_5G!C15</f>
-        <v>0.135745434643157</v>
+        <f>Input3G!C15</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="1">
-        <f>Input4G_5G!C16</f>
-        <v>0.176723300828031</v>
+        <f>Input3G!C16</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="1">
-        <f>Input4G_5G!C17</f>
-        <v>0.29557853355382702</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="1">
-        <f>Input4G_5G!C18</f>
-        <v>0.127877072286533</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="33" t="str">
-        <f>Input4G_5G!A24</f>
-        <v>Vodafone:input\VF BMT Car pk UMTS.FMT</v>
-      </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="35"/>
+        <f>Input3G!C17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="32" t="str">
+        <f>Input3G!A23</f>
+        <v>Eir:input\ccd eir UMTS L1.FMT</v>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="34"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="2" t="s">
-        <v>9</v>
+      <c r="B23" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" s="1">
+        <f>Input3G!C20</f>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="26"/>
+      <c r="B24" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="25"/>
       <c r="D24" s="1">
-        <f>Input4G_5G!C21</f>
-        <v>0.43500803314481401</v>
+        <f>Input3G!C21</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="1">
-        <f>Input4G_5G!C22</f>
-        <v>0.56499196685518505</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="22" t="str">
-        <f>Input4G_5G!A24</f>
-        <v>Vodafone:input\VF BMT Car pk UMTS.FMT</v>
-      </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24"/>
+      <c r="B25" s="21" t="str">
+        <f>Input3G!A23</f>
+        <v>Eir:input\ccd eir UMTS L1.FMT</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>